<commit_message>
test: update input files test CASE_1_ITER_like_LTS.
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_1_ITER_like_LTS/conductor_definition.xlsx
+++ b/TDD_examples/CASE_1_ITER_like_LTS/conductor_definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/Description_of_Components/ITER_TF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\TESI\OPENSC2-main\TDD_examples\CASE_1_ITER_like_LTS\conductor1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{A465B267-904C-4BA0-BAE8-C9CE753C6ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E51C37E6-A345-434F-8463-467CCE147B54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D94EA47-08EF-4482-B4F9-42992E740E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t>XLENGTH</t>
   </si>
@@ -88,24 +88,12 @@
     <t>EXTERNAL_HEAT</t>
   </si>
   <si>
-    <t>bfield.xlsx</t>
-  </si>
-  <si>
     <t>EXTERNAL_ALPHAB</t>
   </si>
   <si>
     <t>EXTERNAL_STRAIN</t>
   </si>
   <si>
-    <t>alphab_dummy.xlsx</t>
-  </si>
-  <si>
-    <t>strain_dummy.xlsx</t>
-  </si>
-  <si>
-    <t>Q_file_dummy.xlsx</t>
-  </si>
-  <si>
     <t>MAXNOD</t>
   </si>
   <si>
@@ -115,9 +103,6 @@
     <t>IOP0_TOT</t>
   </si>
   <si>
-    <t>I_file_dummy.xlsx</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -133,9 +118,6 @@
     <t>EXTERNAL_FLOW</t>
   </si>
   <si>
-    <t>flow_dummy.xlsx</t>
-  </si>
-  <si>
     <t>TAUDET</t>
   </si>
   <si>
@@ -211,9 +193,6 @@
     <t>EXTERNAL_GRID</t>
   </si>
   <si>
-    <t>spatial_discretization.xlsx</t>
-  </si>
-  <si>
     <t>custom file name, extension can be xlsx, dat, csv or tsv. Possibility to define a single file with the spatial discretizations for all the conducrors or a file for each conductor (in the last case use different names for the files). No need to have the same extension!</t>
   </si>
   <si>
@@ -269,6 +248,9 @@
   </si>
   <si>
     <t>maximum number of nodes for conductor spatial discretization</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -435,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -479,7 +461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -777,24 +759,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="8"/>
+    <col min="1" max="1" width="20.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -807,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="C2" s="1"/>
       <c r="D2" s="20"/>
@@ -816,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -838,185 +820,185 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
-        <v>30</v>
-      </c>
       <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>28</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" s="26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1030,24 +1012,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="16.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
@@ -1061,13 +1043,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E2" s="19">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1089,7 +1071,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1097,84 +1079,84 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E5" s="29">
         <v>4.3200000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E6" s="29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E7" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E8" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>4</v>
       </c>
@@ -1182,48 +1164,48 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
@@ -1231,14 +1213,14 @@
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>13</v>
       </c>
@@ -1246,50 +1228,50 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>12</v>
       </c>
@@ -1297,16 +1279,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>11</v>
       </c>
@@ -1314,130 +1296,130 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D18" s="15" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E18" s="3">
         <v>10001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="D21" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E21" s="11" t="str">
         <f>E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="D22" s="18" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E23" s="9">
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E24" s="9">
         <v>0.5</v>
@@ -1458,20 +1440,20 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="30" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>

</xml_diff>